<commit_message>
Reset project to start.
</commit_message>
<xml_diff>
--- a/Examples/Studio/EllipsoidMultipleDomain/ellipsoid_md_example.xlsx
+++ b/Examples/Studio/EllipsoidMultipleDomain/ellipsoid_md_example.xlsx
@@ -1,31 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="Calc" lastEdited="140728898420738" lowestEdited="2" rupBuild="4393318016"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="groom" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="optimize" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="analysis" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="studio" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="project" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="data" sheetId="1" r:id="rId2"/>
+    <sheet name="groom" sheetId="2" r:id="rId3"/>
+    <sheet name="optimize" sheetId="3" r:id="rId4"/>
+    <sheet name="analysis" sheetId="4" r:id="rId5"/>
+    <sheet name="studio" sheetId="5" r:id="rId6"/>
+    <sheet name="project" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="32176535295320844" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="84">
   <si>
     <t xml:space="preserve">segmentation_domain1</t>
   </si>
@@ -272,6 +266,19 @@
   </si>
   <si>
     <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t>&lt;!DOCTYPE HTML PUBLIC "-//W3C//DTD HTML 4.0//EN" "http://www.w3.org/TR/REC-html40/strict.dtd"&gt;
+&lt;html&gt;&lt;head&gt;&lt;meta name="qrichtext" content="1" /&gt;&lt;style type="text/css"&gt;
+p, li { white-space: pre-wrap; }
+&lt;/style&gt;&lt;/head&gt;&lt;body style=" font-family:'.AppleSystemUIFont'; font-size:13pt; font-weight:400; font-style:normal;"&gt;
+&lt;p style="-qt-paragraph-type:empty; margin-top:0px; margin-bottom:0px; margin-left:0px; margin-right:0px; -qt-block-indent:0; text-indent:0px; font-family:'Noto Sans'; font-size:11pt;"&gt;&lt;br /&gt;&lt;/p&gt;&lt;/body&gt;&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>Original</t>
   </si>
 </sst>
 </file>
@@ -286,7 +293,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -313,7 +319,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -321,73 +327,62 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="6">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="bottom" horizontal="general" textRotation="0" indent="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="1" applyBorder="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="1" applyBorder="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="1" applyBorder="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="1" applyBorder="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="1" applyBorder="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0"/>
+      <protection locked="1" hidden="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5898" defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="52.58"/>
+    <col min="1" max="1" width="52.58" style="0" customWidth="1"/>
+    <col min="2" max="2" width="52.58" style="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" customFormat="0" ht="12.8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -395,35 +390,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <printOptions gridLines="0"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.052778" bottom="1.052778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -431,19 +426,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView topLeftCell="A1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" customFormat="0" ht="15">
       <c r="A1" s="0" t="s">
         <v>8</v>
       </c>
@@ -454,7 +450,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:3" customFormat="0" ht="15">
       <c r="A2" s="0" t="s">
         <v>11</v>
       </c>
@@ -465,7 +461,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:3" customFormat="0" ht="15">
       <c r="A3" s="0" t="s">
         <v>13</v>
       </c>
@@ -476,7 +472,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:3" customFormat="0" ht="15">
       <c r="A4" s="0" t="s">
         <v>15</v>
       </c>
@@ -487,7 +483,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:3" customFormat="0" ht="15">
       <c r="A5" s="0" t="s">
         <v>16</v>
       </c>
@@ -498,7 +494,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:3" customFormat="0" ht="15">
       <c r="A6" s="0" t="s">
         <v>18</v>
       </c>
@@ -509,7 +505,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:3" customFormat="0" ht="15">
       <c r="A7" s="0" t="s">
         <v>20</v>
       </c>
@@ -520,7 +516,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:3" customFormat="0" ht="15">
       <c r="A8" s="0" t="s">
         <v>21</v>
       </c>
@@ -531,7 +527,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:3" customFormat="0" ht="15">
       <c r="A9" s="0" t="s">
         <v>22</v>
       </c>
@@ -542,7 +538,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:3" customFormat="0" ht="15">
       <c r="A10" s="0" t="s">
         <v>24</v>
       </c>
@@ -553,7 +549,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:3" customFormat="0" ht="15">
       <c r="A11" s="0" t="s">
         <v>25</v>
       </c>
@@ -564,7 +560,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:3" customFormat="0" ht="15">
       <c r="A12" s="0" t="s">
         <v>26</v>
       </c>
@@ -575,7 +571,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:3" customFormat="0" ht="15">
       <c r="A13" s="0" t="s">
         <v>27</v>
       </c>
@@ -586,7 +582,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:3" customFormat="0" ht="15">
       <c r="A14" s="0" t="s">
         <v>29</v>
       </c>
@@ -597,7 +593,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:3" customFormat="0" ht="15">
       <c r="A15" s="0" t="s">
         <v>30</v>
       </c>
@@ -608,7 +604,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:3" customFormat="0" ht="15">
       <c r="A16" s="0" t="s">
         <v>32</v>
       </c>
@@ -619,7 +615,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:3" customFormat="0" ht="15">
       <c r="A17" s="0" t="s">
         <v>33</v>
       </c>
@@ -630,7 +626,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:3" customFormat="0" ht="15">
       <c r="A18" s="0" t="s">
         <v>35</v>
       </c>
@@ -641,7 +637,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:3" customFormat="0" ht="15">
       <c r="A19" s="0" t="s">
         <v>36</v>
       </c>
@@ -653,30 +649,28 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <printOptions gridLines="0"/>
+  <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView topLeftCell="A1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" customFormat="0" ht="15">
       <c r="A1" s="0" t="s">
         <v>8</v>
       </c>
@@ -684,7 +678,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" customFormat="0" ht="15">
       <c r="A2" s="0" t="s">
         <v>38</v>
       </c>
@@ -692,7 +686,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:2" customFormat="0" ht="15">
       <c r="A3" s="0" t="s">
         <v>40</v>
       </c>
@@ -700,7 +694,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:2" customFormat="0" ht="15">
       <c r="A4" s="0" t="s">
         <v>42</v>
       </c>
@@ -708,7 +702,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:2" customFormat="0" ht="15">
       <c r="A5" s="0" t="s">
         <v>43</v>
       </c>
@@ -716,7 +710,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:2" customFormat="0" ht="15">
       <c r="A6" s="0" t="s">
         <v>45</v>
       </c>
@@ -724,7 +718,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:2" customFormat="0" ht="15">
       <c r="A7" s="0" t="s">
         <v>46</v>
       </c>
@@ -732,7 +726,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:2" customFormat="0" ht="15">
       <c r="A8" s="0" t="s">
         <v>48</v>
       </c>
@@ -740,7 +734,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:2" customFormat="0" ht="15">
       <c r="A9" s="0" t="s">
         <v>49</v>
       </c>
@@ -748,7 +742,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:2" customFormat="0" ht="15">
       <c r="A10" s="0" t="s">
         <v>51</v>
       </c>
@@ -756,7 +750,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:2" customFormat="0" ht="15">
       <c r="A11" s="0" t="s">
         <v>52</v>
       </c>
@@ -764,7 +758,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:2" customFormat="0" ht="15">
       <c r="A12" s="0" t="s">
         <v>54</v>
       </c>
@@ -772,7 +766,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:2" customFormat="0" ht="15">
       <c r="A13" s="0" t="s">
         <v>55</v>
       </c>
@@ -780,7 +774,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:2" customFormat="0" ht="15">
       <c r="A14" s="0" t="s">
         <v>56</v>
       </c>
@@ -788,7 +782,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:2" customFormat="0" ht="15">
       <c r="A15" s="0" t="s">
         <v>57</v>
       </c>
@@ -796,7 +790,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:2" customFormat="0" ht="15">
       <c r="A16" s="0" t="s">
         <v>58</v>
       </c>
@@ -804,7 +798,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:2" customFormat="0" ht="15">
       <c r="A17" s="0" t="s">
         <v>60</v>
       </c>
@@ -812,7 +806,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:2" customFormat="0" ht="15">
       <c r="A18" s="0" t="s">
         <v>61</v>
       </c>
@@ -821,30 +815,28 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <printOptions gridLines="0"/>
+  <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView topLeftCell="A1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" customFormat="0" ht="15">
       <c r="A1" s="0" t="s">
         <v>8</v>
       </c>
@@ -852,7 +844,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" customFormat="0" ht="15">
       <c r="A2" s="0" t="s">
         <v>62</v>
       </c>
@@ -860,7 +852,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:2" customFormat="0" ht="15">
       <c r="A3" s="0" t="s">
         <v>64</v>
       </c>
@@ -868,7 +860,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:2" customFormat="0" ht="15">
       <c r="A4" s="0" t="s">
         <v>66</v>
       </c>
@@ -877,30 +869,28 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <printOptions gridLines="0"/>
+  <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView topLeftCell="A1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" customFormat="0" ht="15">
       <c r="A1" s="0" t="s">
         <v>8</v>
       </c>
@@ -908,7 +898,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" customFormat="0" ht="15">
       <c r="A2" s="0" t="s">
         <v>68</v>
       </c>
@@ -916,7 +906,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:2" customFormat="0" ht="15">
       <c r="A3" s="0" t="s">
         <v>70</v>
       </c>
@@ -924,63 +914,61 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:2" customFormat="0" ht="15">
       <c r="A4" s="0" t="s">
         <v>72</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" customFormat="0" ht="15">
       <c r="A5" s="0" t="s">
         <v>74</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" customFormat="0" ht="15">
       <c r="A6" s="0" t="s">
         <v>76</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" customFormat="0" ht="15">
       <c r="A7" s="0" t="s">
         <v>78</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <printOptions gridLines="0"/>
+  <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView topLeftCell="A1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" customFormat="0" ht="15">
       <c r="A1" s="0" t="s">
         <v>8</v>
       </c>
@@ -988,7 +976,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" customFormat="0" ht="15">
       <c r="A2" s="0" t="s">
         <v>79</v>
       </c>
@@ -997,12 +985,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <printOptions gridLines="0"/>
+  <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>